<commit_message>
Mac-Local-TradingModel / Temp for 2021.11.14
</commit_message>
<xml_diff>
--- a/TEMP_TradingModel_TradingHistory.xlsx
+++ b/TEMP_TradingModel_TradingHistory.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>PositionSize</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -642,6 +642,306 @@
       </c>
       <c r="G8" t="n">
         <v>5973</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3035</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>32</v>
+      </c>
+      <c r="F9" t="n">
+        <v>185</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5920</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8155</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>-42</v>
+      </c>
+      <c r="F10" t="n">
+        <v>140.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-5901</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6509</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>-91</v>
+      </c>
+      <c r="F11" t="n">
+        <v>67.3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-6124.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3504</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>43</v>
+      </c>
+      <c r="F12" t="n">
+        <v>138</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5934</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>44510</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6411</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>26</v>
+      </c>
+      <c r="F13" t="n">
+        <v>230</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5980</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>44510</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4739</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>-40</v>
+      </c>
+      <c r="F14" t="n">
+        <v>145.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-5820</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3033</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>180</v>
+      </c>
+      <c r="F15" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6170</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>-117</v>
+      </c>
+      <c r="F16" t="n">
+        <v>47</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-5499</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3588</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>35</v>
+      </c>
+      <c r="F17" t="n">
+        <v>155</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5425</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3504</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>-43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>132</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-5676</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6104</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>36</v>
+      </c>
+      <c r="F19" t="n">
+        <v>170</v>
+      </c>
+      <c r="G19" t="n">
+        <v>6120</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2436</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>lomg</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>50</v>
+      </c>
+      <c r="F20" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>